<commit_message>
paper update iros / jones
</commit_message>
<xml_diff>
--- a/conference/pagegen/data/faim-18.xlsx
+++ b/conference/pagegen/data/faim-18.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6BD156-AD63-4333-BC06-A586F7F42063}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448D54D1-A76C-4FCA-AEDD-AC660DBAAA9C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AAMAS 2018" sheetId="2" r:id="rId1"/>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DCF7FF2-5513-4694-9A44-0590350F5772}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:E3"/>
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBE9F31-0271-4DD6-92EF-89236D515945}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:E6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>